<commit_message>
chaged sensor boards, INventor 2018 format
</commit_message>
<xml_diff>
--- a/modularHodoscope.xlsx
+++ b/modularHodoscope.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sawaiz\OneDrive\projects\modularHodoscope\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="7" documentId="B4C4100603664A2070CBB031988EBC5112407FB1" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{8576C899-0415-4BE5-92CC-D51B202EF9C2}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="8265"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="8265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -68,7 +69,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
@@ -384,7 +385,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -414,7 +415,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="2">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>

</xml_diff>